<commit_message>
Code Review F2F Done
</commit_message>
<xml_diff>
--- a/1. Login.xlsx
+++ b/1. Login.xlsx
@@ -14,42 +14,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Url</t>
   </si>
   <si>
+    <t>http://gdkwebsvr:4100/</t>
+  </si>
+  <si>
+    <t>Database Connection</t>
+  </si>
+  <si>
+    <t>Server Name</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
     <t>Username</t>
   </si>
   <si>
     <t>Password</t>
   </si>
   <si>
-    <t>http://gdkwebsvr:4100/login</t>
-  </si>
-  <si>
-    <t>kevin.edgar@ad-ins.com</t>
-  </si>
-  <si>
-    <t>Xavier123!</t>
-  </si>
-  <si>
-    <t>Database Connection</t>
-  </si>
-  <si>
-    <t>Server Name</t>
-  </si>
-  <si>
-    <t>Port</t>
-  </si>
-  <si>
-    <t>Database</t>
-  </si>
-  <si>
     <t>jdbc:postgresql://CREATOR_DBSVR</t>
   </si>
   <si>
-    <t>adins_apiaas?currentSchema=esign</t>
+    <t>eendigo_prod_test_deploy_modify?currentSchema=esign</t>
   </si>
   <si>
     <t>sa</t>
@@ -69,8 +63,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -91,6 +85,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -98,8 +115,48 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -115,6 +172,35 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -122,10 +208,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -136,100 +222,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -244,19 +238,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -268,7 +352,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -280,151 +418,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,16 +457,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -488,17 +482,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -537,23 +520,34 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -571,130 +565,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -704,6 +698,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -711,7 +706,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1034,14 +1028,14 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="33.2727272727273" customWidth="1"/>
     <col min="2" max="2" width="23.7272727272727" customWidth="1"/>
-    <col min="3" max="3" width="33.7272727272727" customWidth="1"/>
+    <col min="3" max="3" width="54.4545454545455" customWidth="1"/>
     <col min="4" max="4" width="10.1818181818182" customWidth="1"/>
     <col min="5" max="5" width="10.3636363636364" customWidth="1"/>
     <col min="6" max="6" width="43.3636363636364" customWidth="1"/>
@@ -1051,42 +1045,34 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="5"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="5"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="5"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="5"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
@@ -1100,48 +1086,48 @@
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="A6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="B8" s="8">
+        <v>5432</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="7">
-        <v>5432</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="E8" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -1179,7 +1165,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
@@ -1188,8 +1174,8 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="8" t="s">
-        <v>15</v>
+      <c r="A14" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhancement OTP & New Write to Excel Done
</commit_message>
<xml_diff>
--- a/1. Login.xlsx
+++ b/1. Login.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Url</t>
   </si>
@@ -43,13 +43,16 @@
     <t>jdbc:postgresql://CREATOR_DBSVR</t>
   </si>
   <si>
-    <t>eendigo_prod_test_deploy_modify?currentSchema=esign</t>
+    <t>eendigo_prod_test_deploy_modify_2?currentSchema=esign</t>
   </si>
   <si>
     <t>sa</t>
   </si>
   <si>
     <t>AdIns2021</t>
+  </si>
+  <si>
+    <t>eendigo_prod_test_deploy_modify_2?currentSchema=public</t>
   </si>
   <si>
     <t>CheckDBAPIAAS?(Yes/No)</t>
@@ -64,9 +67,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -85,14 +88,95 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -101,15 +185,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -124,16 +209,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -141,22 +218,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -169,65 +231,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -238,187 +241,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,8 +453,17 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -471,6 +483,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -486,35 +513,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -533,29 +547,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -565,139 +568,138 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1028,7 +1030,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B13" sqref="B13:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="5"/>
@@ -1055,24 +1057,24 @@
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="6"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="6"/>
+      <c r="C3" s="5"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="6"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="6"/>
+      <c r="C4" s="5"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
@@ -1086,13 +1088,13 @@
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6">
@@ -1114,29 +1116,39 @@
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>5432</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7">
+        <v>5432</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6">
@@ -1165,28 +1177,23 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="B13"/>
+      <c r="C13"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="5" t="s">
-        <v>13</v>
+      <c r="A14" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A6:E6"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13">
-      <formula1>"CF4W, FL4W"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Cek OCR KK aja
</commit_message>
<xml_diff>
--- a/1. Login.xlsx
+++ b/1. Login.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Url</t>
   </si>
@@ -43,13 +43,25 @@
     <t>jdbc:postgresql://CREATOR_DBSVR</t>
   </si>
   <si>
-    <t>eendigo_prod_test_deploy_modify_2</t>
+    <t>eendigo_dev</t>
   </si>
   <si>
     <t>sa</t>
   </si>
   <si>
     <t>AdIns2021</t>
+  </si>
+  <si>
+    <t>jdbc:postgresql://pgm-d9j41ftwhk9lepulto.pgsql.ap-southeast-5.rds.aliyuncs.com</t>
+  </si>
+  <si>
+    <t>adins_apiaas_uat</t>
+  </si>
+  <si>
+    <t>qa_view</t>
+  </si>
+  <si>
+    <t>AdIns2022!</t>
   </si>
   <si>
     <t>CheckDBAPIAAS?(Yes/No)</t>
@@ -63,10 +75,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -85,6 +97,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -99,33 +126,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -139,22 +142,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -169,22 +190,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -193,30 +198,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,181 +250,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,16 +460,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -481,7 +502,16 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -502,34 +532,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -547,7 +559,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -565,134 +577,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -704,6 +716,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1027,7 +1042,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="5"/>
@@ -1130,12 +1145,22 @@
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="4"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+    <row r="9" ht="43.5" spans="1:6">
+      <c r="A9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="7">
+        <v>5432</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6">
@@ -1164,7 +1189,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1172,7 +1197,7 @@
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Quantity price fixed and Saldo API (billing system) done
</commit_message>
<xml_diff>
--- a/1. Login.xlsx
+++ b/1. Login.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Url</t>
   </si>
   <si>
     <t>http://gdkwebsvr:4100/</t>
+  </si>
+  <si>
+    <t>http://websvr:8000/</t>
   </si>
   <si>
     <t>Database Connection</t>
@@ -75,10 +78,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -97,18 +100,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -119,8 +138,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -129,6 +149,14 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -142,50 +170,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -204,8 +206,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -221,21 +239,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -250,187 +253,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,25 +463,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -502,16 +496,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -531,17 +516,35 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -559,7 +562,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -577,139 +580,141 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1042,7 +1047,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="5"/>
@@ -1076,17 +1081,19 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="5"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="5"/>
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="5"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="5"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
@@ -1100,66 +1107,66 @@
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="A6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="7">
+        <v>9</v>
+      </c>
+      <c r="B8" s="9">
         <v>5432</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" ht="43.5" spans="1:6">
-      <c r="A9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="7">
+      <c r="A9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="9">
         <v>5432</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -1189,7 +1196,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1197,7 +1204,7 @@
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Balikan AT 49 Done
</commit_message>
<xml_diff>
--- a/1. Login.xlsx
+++ b/1. Login.xlsx
@@ -100,6 +100,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -107,19 +116,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -138,6 +146,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -146,6 +169,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -156,36 +208,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -200,7 +223,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -208,37 +231,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,31 +253,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,151 +379,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,6 +458,35 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -492,15 +521,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -512,24 +532,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -551,18 +553,16 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -580,139 +580,138 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1047,7 +1046,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="5"/>
@@ -1071,7 +1070,7 @@
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4"/>
@@ -1081,19 +1080,19 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="5" t="s">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="6"/>
+      <c r="C3" s="5"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="7"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="7"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
@@ -1107,13 +1106,13 @@
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6">
@@ -1138,7 +1137,7 @@
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>5432</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1153,10 +1152,10 @@
       <c r="F8" s="2"/>
     </row>
     <row r="9" ht="43.5" spans="1:6">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>5432</v>
       </c>
       <c r="C9" s="4" t="s">

</xml_diff>

<commit_message>
AT49 rework for code Review
</commit_message>
<xml_diff>
--- a/1. Login.xlsx
+++ b/1. Login.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Url</t>
   </si>
@@ -28,7 +28,7 @@
     <t>http://gdkwebsvr:4100/</t>
   </si>
   <si>
-    <t>http://websvr:8000/</t>
+    <t>http://websvr:4600/</t>
   </si>
   <si>
     <t>ADMESIGN</t>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>AdIns2022!</t>
+  </si>
+  <si>
+    <t>eendigo_dev_uat</t>
   </si>
   <si>
     <t>CheckDBAPIAAS?(Yes/No)</t>
@@ -107,7 +110,107 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -121,16 +224,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -138,15 +233,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -154,97 +248,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,49 +262,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,61 +412,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -379,67 +442,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -477,11 +480,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -497,36 +539,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -556,19 +568,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -586,139 +589,138 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1052,7 +1054,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="5"/>
@@ -1083,8 +1085,8 @@
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="3"/>
@@ -1104,8 +1106,8 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="A4" s="5"/>
+      <c r="C4" s="5"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
@@ -1119,13 +1121,13 @@
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6">
@@ -1147,47 +1149,57 @@
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>5432</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" ht="43.5" spans="1:6">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>5432</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="A10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="7">
+        <v>5432</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6">
@@ -1208,15 +1220,15 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="5" t="s">
-        <v>20</v>
+      <c r="A14" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>